<commit_message>
adding more excel functions
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Users.xlsx
+++ b/ProjectTesting/Excel/Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Biscuits\source\repos\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333D4CAD-3565-400E-9595-02F0E0880F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B26786C-3D25-4154-87CC-5BE027244515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="17010" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>UserName</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Max</t>
-  </si>
-  <si>
-    <t>Maxim</t>
   </si>
 </sst>
 </file>
@@ -394,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -438,11 +435,6 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixing readRange and writeRange functions
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Users.xlsx
+++ b/ProjectTesting/Excel/Users.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayh\Documents\Visual Studio 2022\Projects\ProjectTesting\ProjectTesting\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Biscuits\source\repos\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FCDBB4-EF36-4C3F-AB66-1DF26033549D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981A987E-BBCD-4AC6-BBBA-9C722EEB7D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="17010" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>UserName</t>
   </si>
@@ -42,7 +42,10 @@
     <t>Max</t>
   </si>
   <si>
-    <t>something</t>
+    <t>max</t>
+  </si>
+  <si>
+    <t>123321</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -438,9 +441,12 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new signup and pictures
</commit_message>
<xml_diff>
--- a/ProjectTesting/Excel/Users.xlsx
+++ b/ProjectTesting/Excel/Users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayh\Documents\Visual Studio 2022\Projects\ProjectTesting\ProjectTesting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BCAA19-27AE-4224-B863-BD7BC8457F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7BC07F-DCEE-4D1C-86A0-263F95ABB3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>UserName</t>
   </si>
@@ -42,10 +42,16 @@
     <t>Max</t>
   </si>
   <si>
-    <t>max</t>
+    <t>Dave</t>
   </si>
   <si>
-    <t>123321</t>
+    <t>Dave&amp;123</t>
+  </si>
+  <si>
+    <t>323232</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -108,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -116,6 +122,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -397,65 +408,1261 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D401"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="20.7109375" style="3" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
+    <col min="3" max="3" width="20.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3">
         <v>1234</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="6">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3">
         <v>9999</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="6">
+        <v>207623</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3">
         <v>1235</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="6">
+        <v>291232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
+      <c r="C5" s="6" t="s">
+        <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C50" s="6"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C51" s="6"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C52" s="6"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C53" s="6"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C54" s="6"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C55" s="6"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C56" s="6"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C57" s="6"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C58" s="6"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C59" s="6"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C60" s="6"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C61" s="6"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C62" s="6"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C63" s="6"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C64" s="6"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C65" s="6"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C66" s="6"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C67" s="6"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C68" s="6"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C69" s="6"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C70" s="6"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C71" s="6"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C72" s="6"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C73" s="6"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C74" s="6"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C75" s="6"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C76" s="6"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C77" s="6"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C78" s="6"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C79" s="6"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C80" s="6"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C81" s="6"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C82" s="6"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C83" s="6"/>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C84" s="6"/>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C85" s="6"/>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C86" s="6"/>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C87" s="6"/>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C88" s="6"/>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C89" s="6"/>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C90" s="6"/>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C91" s="6"/>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C92" s="6"/>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C93" s="6"/>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C94" s="6"/>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C95" s="6"/>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C96" s="6"/>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C97" s="6"/>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C98" s="6"/>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C99" s="6"/>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C100" s="6"/>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C101" s="6"/>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C102" s="6"/>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C103" s="6"/>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C104" s="6"/>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C105" s="6"/>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C106" s="6"/>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C107" s="6"/>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C108" s="6"/>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C109" s="6"/>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C110" s="6"/>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C111" s="6"/>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C112" s="6"/>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C113" s="6"/>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C114" s="6"/>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C115" s="6"/>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C116" s="6"/>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C117" s="6"/>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C118" s="6"/>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C119" s="6"/>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C120" s="6"/>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C121" s="6"/>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C122" s="6"/>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C123" s="6"/>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C124" s="6"/>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C125" s="6"/>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C126" s="6"/>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C127" s="6"/>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C128" s="6"/>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C129" s="6"/>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C130" s="6"/>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C131" s="6"/>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C132" s="6"/>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C133" s="6"/>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C134" s="6"/>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C135" s="6"/>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C136" s="6"/>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C137" s="6"/>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C138" s="6"/>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C139" s="6"/>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C140" s="6"/>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C141" s="6"/>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C142" s="6"/>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C143" s="6"/>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C144" s="6"/>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C145" s="6"/>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C146" s="6"/>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C147" s="6"/>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C148" s="6"/>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C149" s="6"/>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C150" s="6"/>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C151" s="6"/>
+    </row>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C152" s="6"/>
+    </row>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C153" s="6"/>
+    </row>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C154" s="6"/>
+    </row>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C155" s="6"/>
+    </row>
+    <row r="156" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C156" s="6"/>
+    </row>
+    <row r="157" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C157" s="6"/>
+    </row>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C158" s="6"/>
+    </row>
+    <row r="159" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C159" s="6"/>
+    </row>
+    <row r="160" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C160" s="6"/>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C161" s="6"/>
+    </row>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C162" s="6"/>
+    </row>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C163" s="6"/>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C164" s="6"/>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C165" s="6"/>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C166" s="6"/>
+    </row>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C167" s="6"/>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C168" s="6"/>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C169" s="6"/>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C170" s="6"/>
+    </row>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C171" s="6"/>
+    </row>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C172" s="6"/>
+    </row>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C173" s="6"/>
+    </row>
+    <row r="174" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C174" s="6"/>
+    </row>
+    <row r="175" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C175" s="6"/>
+    </row>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C176" s="6"/>
+    </row>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C177" s="6"/>
+    </row>
+    <row r="178" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C178" s="6"/>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C179" s="6"/>
+    </row>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C180" s="6"/>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C181" s="6"/>
+    </row>
+    <row r="182" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C182" s="6"/>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C183" s="6"/>
+    </row>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C184" s="6"/>
+    </row>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C185" s="6"/>
+    </row>
+    <row r="186" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C186" s="6"/>
+    </row>
+    <row r="187" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C187" s="6"/>
+    </row>
+    <row r="188" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C188" s="6"/>
+    </row>
+    <row r="189" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C189" s="6"/>
+    </row>
+    <row r="190" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C190" s="6"/>
+    </row>
+    <row r="191" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C191" s="6"/>
+    </row>
+    <row r="192" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C192" s="6"/>
+    </row>
+    <row r="193" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C193" s="6"/>
+    </row>
+    <row r="194" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C194" s="6"/>
+    </row>
+    <row r="195" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C195" s="6"/>
+    </row>
+    <row r="196" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C196" s="6"/>
+    </row>
+    <row r="197" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C197" s="6"/>
+    </row>
+    <row r="198" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C198" s="6"/>
+    </row>
+    <row r="199" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C199" s="6"/>
+    </row>
+    <row r="200" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C200" s="6"/>
+    </row>
+    <row r="201" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C201" s="6"/>
+    </row>
+    <row r="202" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C202" s="6"/>
+    </row>
+    <row r="203" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C203" s="6"/>
+    </row>
+    <row r="204" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C204" s="6"/>
+    </row>
+    <row r="205" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C205" s="6"/>
+    </row>
+    <row r="206" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C206" s="6"/>
+    </row>
+    <row r="207" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C207" s="6"/>
+    </row>
+    <row r="208" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C208" s="6"/>
+    </row>
+    <row r="209" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C209" s="6"/>
+    </row>
+    <row r="210" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C210" s="6"/>
+    </row>
+    <row r="211" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C211" s="6"/>
+    </row>
+    <row r="212" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C212" s="6"/>
+    </row>
+    <row r="213" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C213" s="6"/>
+    </row>
+    <row r="214" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C214" s="6"/>
+    </row>
+    <row r="215" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C215" s="6"/>
+    </row>
+    <row r="216" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C216" s="6"/>
+    </row>
+    <row r="217" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C217" s="6"/>
+    </row>
+    <row r="218" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C218" s="6"/>
+    </row>
+    <row r="219" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C219" s="6"/>
+    </row>
+    <row r="220" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C220" s="6"/>
+    </row>
+    <row r="221" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C221" s="6"/>
+    </row>
+    <row r="222" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C222" s="6"/>
+    </row>
+    <row r="223" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C223" s="6"/>
+    </row>
+    <row r="224" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C224" s="6"/>
+    </row>
+    <row r="225" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C225" s="6"/>
+    </row>
+    <row r="226" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C226" s="6"/>
+    </row>
+    <row r="227" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C227" s="6"/>
+    </row>
+    <row r="228" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C228" s="6"/>
+    </row>
+    <row r="229" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C229" s="6"/>
+    </row>
+    <row r="230" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C230" s="6"/>
+    </row>
+    <row r="231" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C231" s="6"/>
+    </row>
+    <row r="232" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C232" s="6"/>
+    </row>
+    <row r="233" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C233" s="6"/>
+    </row>
+    <row r="234" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C234" s="6"/>
+    </row>
+    <row r="235" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C235" s="6"/>
+    </row>
+    <row r="236" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C236" s="6"/>
+    </row>
+    <row r="237" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C237" s="6"/>
+    </row>
+    <row r="238" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C238" s="6"/>
+    </row>
+    <row r="239" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C239" s="6"/>
+    </row>
+    <row r="240" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C240" s="6"/>
+    </row>
+    <row r="241" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C241" s="6"/>
+    </row>
+    <row r="242" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C242" s="6"/>
+    </row>
+    <row r="243" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C243" s="6"/>
+    </row>
+    <row r="244" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C244" s="6"/>
+    </row>
+    <row r="245" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C245" s="6"/>
+    </row>
+    <row r="246" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C246" s="6"/>
+    </row>
+    <row r="247" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C247" s="6"/>
+    </row>
+    <row r="248" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C248" s="6"/>
+    </row>
+    <row r="249" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C249" s="6"/>
+    </row>
+    <row r="250" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C250" s="6"/>
+    </row>
+    <row r="251" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C251" s="6"/>
+    </row>
+    <row r="252" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C252" s="6"/>
+    </row>
+    <row r="253" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C253" s="6"/>
+    </row>
+    <row r="254" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C254" s="6"/>
+    </row>
+    <row r="255" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C255" s="6"/>
+    </row>
+    <row r="256" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C256" s="6"/>
+    </row>
+    <row r="257" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C257" s="6"/>
+    </row>
+    <row r="258" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C258" s="6"/>
+    </row>
+    <row r="259" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C259" s="6"/>
+    </row>
+    <row r="260" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C260" s="6"/>
+    </row>
+    <row r="261" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C261" s="6"/>
+    </row>
+    <row r="262" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C262" s="6"/>
+    </row>
+    <row r="263" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C263" s="6"/>
+    </row>
+    <row r="264" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C264" s="6"/>
+    </row>
+    <row r="265" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C265" s="6"/>
+    </row>
+    <row r="266" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C266" s="6"/>
+    </row>
+    <row r="267" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C267" s="6"/>
+    </row>
+    <row r="268" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C268" s="6"/>
+    </row>
+    <row r="269" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C269" s="6"/>
+    </row>
+    <row r="270" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C270" s="6"/>
+    </row>
+    <row r="271" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C271" s="6"/>
+    </row>
+    <row r="272" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C272" s="6"/>
+    </row>
+    <row r="273" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C273" s="6"/>
+    </row>
+    <row r="274" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C274" s="6"/>
+    </row>
+    <row r="275" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C275" s="6"/>
+    </row>
+    <row r="276" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C276" s="6"/>
+    </row>
+    <row r="277" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C277" s="6"/>
+    </row>
+    <row r="278" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C278" s="6"/>
+    </row>
+    <row r="279" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C279" s="6"/>
+    </row>
+    <row r="280" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C280" s="6"/>
+    </row>
+    <row r="281" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C281" s="6"/>
+    </row>
+    <row r="282" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C282" s="6"/>
+    </row>
+    <row r="283" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C283" s="6"/>
+    </row>
+    <row r="284" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C284" s="6"/>
+    </row>
+    <row r="285" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C285" s="6"/>
+    </row>
+    <row r="286" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C286" s="6"/>
+    </row>
+    <row r="287" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C287" s="6"/>
+    </row>
+    <row r="288" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C288" s="6"/>
+    </row>
+    <row r="289" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C289" s="6"/>
+    </row>
+    <row r="290" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C290" s="6"/>
+    </row>
+    <row r="291" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C291" s="6"/>
+    </row>
+    <row r="292" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C292" s="6"/>
+    </row>
+    <row r="293" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C293" s="6"/>
+    </row>
+    <row r="294" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C294" s="6"/>
+    </row>
+    <row r="295" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C295" s="6"/>
+    </row>
+    <row r="296" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C296" s="6"/>
+    </row>
+    <row r="297" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C297" s="5"/>
+    </row>
+    <row r="298" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C298" s="5"/>
+    </row>
+    <row r="299" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C299" s="5"/>
+    </row>
+    <row r="300" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C300" s="5"/>
+    </row>
+    <row r="301" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C301" s="5"/>
+    </row>
+    <row r="302" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C302" s="5"/>
+    </row>
+    <row r="303" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C303" s="5"/>
+    </row>
+    <row r="304" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C304" s="5"/>
+    </row>
+    <row r="305" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C305" s="5"/>
+    </row>
+    <row r="306" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C306" s="5"/>
+    </row>
+    <row r="307" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C307" s="5"/>
+    </row>
+    <row r="308" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C308" s="5"/>
+    </row>
+    <row r="309" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C309" s="5"/>
+    </row>
+    <row r="310" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C310" s="5"/>
+    </row>
+    <row r="311" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C311" s="5"/>
+    </row>
+    <row r="312" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C312" s="5"/>
+    </row>
+    <row r="313" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C313" s="5"/>
+    </row>
+    <row r="314" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C314" s="5"/>
+    </row>
+    <row r="315" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C315" s="5"/>
+    </row>
+    <row r="316" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C316" s="5"/>
+    </row>
+    <row r="317" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C317" s="5"/>
+    </row>
+    <row r="318" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C318" s="5"/>
+    </row>
+    <row r="319" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C319" s="5"/>
+    </row>
+    <row r="320" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C320" s="5"/>
+    </row>
+    <row r="321" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C321" s="5"/>
+    </row>
+    <row r="322" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C322" s="5"/>
+    </row>
+    <row r="323" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C323" s="5"/>
+    </row>
+    <row r="324" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C324" s="5"/>
+    </row>
+    <row r="325" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C325" s="5"/>
+    </row>
+    <row r="326" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C326" s="5"/>
+    </row>
+    <row r="327" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C327" s="5"/>
+    </row>
+    <row r="328" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C328" s="5"/>
+    </row>
+    <row r="329" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C329" s="5"/>
+    </row>
+    <row r="330" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C330" s="5"/>
+    </row>
+    <row r="331" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C331" s="5"/>
+    </row>
+    <row r="332" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C332" s="5"/>
+    </row>
+    <row r="333" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C333" s="5"/>
+    </row>
+    <row r="334" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C334" s="5"/>
+    </row>
+    <row r="335" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C335" s="5"/>
+    </row>
+    <row r="336" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C336" s="5"/>
+    </row>
+    <row r="337" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C337" s="5"/>
+    </row>
+    <row r="338" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C338" s="5"/>
+    </row>
+    <row r="339" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C339" s="5"/>
+    </row>
+    <row r="340" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C340" s="5"/>
+    </row>
+    <row r="341" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C341" s="5"/>
+    </row>
+    <row r="342" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C342" s="5"/>
+    </row>
+    <row r="343" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C343" s="5"/>
+    </row>
+    <row r="344" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C344" s="5"/>
+    </row>
+    <row r="345" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C345" s="5"/>
+    </row>
+    <row r="346" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C346" s="5"/>
+    </row>
+    <row r="347" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C347" s="5"/>
+    </row>
+    <row r="348" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C348" s="5"/>
+    </row>
+    <row r="349" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C349" s="5"/>
+    </row>
+    <row r="350" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C350" s="5"/>
+    </row>
+    <row r="351" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C351" s="5"/>
+    </row>
+    <row r="352" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C352" s="5"/>
+    </row>
+    <row r="353" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C353" s="5"/>
+    </row>
+    <row r="354" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C354" s="5"/>
+    </row>
+    <row r="355" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C355" s="5"/>
+    </row>
+    <row r="356" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C356" s="5"/>
+    </row>
+    <row r="357" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C357" s="5"/>
+    </row>
+    <row r="358" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C358" s="5"/>
+    </row>
+    <row r="359" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C359" s="5"/>
+    </row>
+    <row r="360" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C360" s="5"/>
+    </row>
+    <row r="361" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C361" s="5"/>
+    </row>
+    <row r="362" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C362" s="5"/>
+    </row>
+    <row r="363" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C363" s="5"/>
+    </row>
+    <row r="364" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C364" s="5"/>
+    </row>
+    <row r="365" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C365" s="5"/>
+    </row>
+    <row r="366" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C366" s="5"/>
+    </row>
+    <row r="367" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C367" s="5"/>
+    </row>
+    <row r="368" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C368" s="5"/>
+    </row>
+    <row r="369" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C369" s="5"/>
+    </row>
+    <row r="370" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C370" s="5"/>
+    </row>
+    <row r="371" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C371" s="5"/>
+    </row>
+    <row r="372" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C372" s="5"/>
+    </row>
+    <row r="373" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C373" s="5"/>
+    </row>
+    <row r="374" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C374" s="5"/>
+    </row>
+    <row r="375" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C375" s="5"/>
+    </row>
+    <row r="376" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C376" s="5"/>
+    </row>
+    <row r="377" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C377" s="5"/>
+    </row>
+    <row r="378" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C378" s="5"/>
+    </row>
+    <row r="379" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C379" s="5"/>
+    </row>
+    <row r="380" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C380" s="5"/>
+    </row>
+    <row r="381" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C381" s="5"/>
+    </row>
+    <row r="382" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C382" s="5"/>
+    </row>
+    <row r="383" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C383" s="5"/>
+    </row>
+    <row r="384" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C384" s="5"/>
+    </row>
+    <row r="385" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C385" s="5"/>
+    </row>
+    <row r="386" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C386" s="5"/>
+    </row>
+    <row r="387" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C387" s="5"/>
+    </row>
+    <row r="388" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C388" s="5"/>
+    </row>
+    <row r="389" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C389" s="5"/>
+    </row>
+    <row r="390" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C390" s="5"/>
+    </row>
+    <row r="391" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C391" s="5"/>
+    </row>
+    <row r="392" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C392" s="5"/>
+    </row>
+    <row r="393" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C393" s="5"/>
+    </row>
+    <row r="394" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C394" s="5"/>
+    </row>
+    <row r="395" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C395" s="5"/>
+    </row>
+    <row r="396" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C396" s="5"/>
+    </row>
+    <row r="397" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C397" s="5"/>
+    </row>
+    <row r="398" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C398" s="5"/>
+    </row>
+    <row r="399" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C399" s="5"/>
+    </row>
+    <row r="400" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C400" s="5"/>
+    </row>
+    <row r="401" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C401" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>